<commit_message>
pago actualizado al 10 de agosto
</commit_message>
<xml_diff>
--- a/DATA/Pagos.xlsx
+++ b/DATA/Pagos.xlsx
@@ -210,19 +210,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -258,15 +252,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -583,9 +574,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="46.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="46.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" hidden="1">
@@ -599,11 +590,11 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" hidden="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -614,7 +605,7 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -625,7 +616,7 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -636,7 +627,7 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -647,7 +638,7 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -658,7 +649,7 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -669,7 +660,7 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -680,7 +671,7 @@
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -691,7 +682,7 @@
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -702,7 +693,7 @@
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -713,7 +704,7 @@
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -724,7 +715,7 @@
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -735,7 +726,7 @@
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -746,7 +737,7 @@
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -757,7 +748,7 @@
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -768,7 +759,7 @@
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -779,7 +770,7 @@
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -790,7 +781,7 @@
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -801,7 +792,7 @@
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -812,7 +803,7 @@
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -823,51 +814,51 @@
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" hidden="1">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" hidden="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" hidden="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75" hidden="1">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -878,7 +869,7 @@
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -889,7 +880,7 @@
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -900,7 +891,7 @@
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -911,7 +902,7 @@
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -922,7 +913,7 @@
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -933,7 +924,7 @@
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -944,7 +935,7 @@
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -955,7 +946,7 @@
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -966,7 +957,7 @@
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -977,7 +968,7 @@
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -988,7 +979,7 @@
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -999,29 +990,29 @@
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75" hidden="1">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" hidden="1">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1032,7 +1023,7 @@
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1043,7 +1034,7 @@
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1054,7 +1045,7 @@
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1065,7 +1056,7 @@
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1076,7 +1067,7 @@
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1087,7 +1078,7 @@
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1098,7 +1089,7 @@
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1109,7 +1100,7 @@
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1120,7 +1111,7 @@
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -1131,7 +1122,7 @@
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -1142,7 +1133,7 @@
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -1153,7 +1144,7 @@
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -1164,7 +1155,7 @@
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -1175,7 +1166,7 @@
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -1186,7 +1177,7 @@
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="2">
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -1197,7 +1188,7 @@
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="2">
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -1208,18 +1199,18 @@
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="2">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" hidden="1">
       <c r="A58" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <v>2</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -1230,7 +1221,7 @@
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <v>2</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -1241,7 +1232,7 @@
       <c r="A60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="2">
         <v>2</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -1252,7 +1243,7 @@
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="2">
         <v>2</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -1263,7 +1254,7 @@
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="2">
         <v>2</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -1274,7 +1265,7 @@
       <c r="A63" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="2">
         <v>2</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -1285,7 +1276,7 @@
       <c r="A64" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="2">
         <v>2</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -1296,7 +1287,7 @@
       <c r="A65" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="2">
         <v>2</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -1307,7 +1298,7 @@
       <c r="A66" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="2">
         <v>2</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -1318,7 +1309,7 @@
       <c r="A67" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="2">
         <v>2</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -1329,7 +1320,7 @@
       <c r="A68" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="2">
         <v>2</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -1340,7 +1331,7 @@
       <c r="A69" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="2">
         <v>2</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -1351,7 +1342,7 @@
       <c r="A70" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="2">
         <v>2</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -1362,7 +1353,7 @@
       <c r="A71" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="2">
         <v>2</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -1373,7 +1364,7 @@
       <c r="A72" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="2">
         <v>2</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -1384,7 +1375,7 @@
       <c r="A73" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="2">
         <v>2</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -1395,7 +1386,7 @@
       <c r="A74" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="2">
         <v>2</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -1406,7 +1397,7 @@
       <c r="A75" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="2">
         <v>2</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -1417,7 +1408,7 @@
       <c r="A76" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="2">
         <v>2</v>
       </c>
       <c r="C76" s="1" t="s">
@@ -1428,7 +1419,7 @@
       <c r="A77" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="2">
         <v>2</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -1439,40 +1430,40 @@
       <c r="A78" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="2">
         <v>2</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75" hidden="1">
       <c r="A79" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="2">
         <v>2</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75" hidden="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="2">
         <v>2</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="2">
         <v>2</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -1483,7 +1474,7 @@
       <c r="A82" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="2">
         <v>2</v>
       </c>
       <c r="C82" s="1" t="s">
@@ -1494,7 +1485,7 @@
       <c r="A83" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="2">
         <v>2</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -1505,7 +1496,7 @@
       <c r="A84" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B84" s="2">
         <v>2</v>
       </c>
       <c r="C84" s="1" t="s">
@@ -1516,7 +1507,7 @@
       <c r="A85" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B85" s="2">
         <v>2</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -1527,7 +1518,7 @@
       <c r="A86" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86" s="2">
         <v>2</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -1538,7 +1529,7 @@
       <c r="A87" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B87" s="2">
         <v>2</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -1549,7 +1540,7 @@
       <c r="A88" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B88" s="2">
         <v>2</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -1560,7 +1551,7 @@
       <c r="A89" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B89" s="2">
         <v>2</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -1571,7 +1562,7 @@
       <c r="A90" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B90" s="2">
         <v>2</v>
       </c>
       <c r="C90" s="1" t="s">
@@ -1582,7 +1573,7 @@
       <c r="A91" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B91" s="2">
         <v>2</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -1593,7 +1584,7 @@
       <c r="A92" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B92" s="2">
         <v>2</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -1604,7 +1595,7 @@
       <c r="A93" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="2">
         <v>2</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -1615,29 +1606,29 @@
       <c r="A94" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="2">
         <v>2</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75" hidden="1">
       <c r="A95" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="2">
         <v>2</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75" hidden="1">
       <c r="A96" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="2">
         <v>2</v>
       </c>
       <c r="C96" s="1" t="s">
@@ -1648,7 +1639,7 @@
       <c r="A97" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="2">
         <v>2</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -1659,7 +1650,7 @@
       <c r="A98" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98" s="2">
         <v>2</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -1670,7 +1661,7 @@
       <c r="A99" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B99" s="2">
         <v>2</v>
       </c>
       <c r="C99" s="1" t="s">
@@ -1681,7 +1672,7 @@
       <c r="A100" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B100" s="2">
         <v>2</v>
       </c>
       <c r="C100" s="1" t="s">
@@ -1692,7 +1683,7 @@
       <c r="A101" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B101" s="2">
         <v>2</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -1703,7 +1694,7 @@
       <c r="A102" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B102" s="3">
+      <c r="B102" s="2">
         <v>2</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -1714,7 +1705,7 @@
       <c r="A103" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B103" s="2">
         <v>2</v>
       </c>
       <c r="C103" s="1" t="s">
@@ -1725,7 +1716,7 @@
       <c r="A104" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B104" s="3">
+      <c r="B104" s="2">
         <v>2</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -1736,7 +1727,7 @@
       <c r="A105" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B105" s="3">
+      <c r="B105" s="2">
         <v>2</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -1747,7 +1738,7 @@
       <c r="A106" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B106" s="3">
+      <c r="B106" s="2">
         <v>2</v>
       </c>
       <c r="C106" s="1" t="s">
@@ -1758,7 +1749,7 @@
       <c r="A107" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B107" s="3">
+      <c r="B107" s="2">
         <v>2</v>
       </c>
       <c r="C107" s="1" t="s">
@@ -1769,7 +1760,7 @@
       <c r="A108" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108" s="2">
         <v>2</v>
       </c>
       <c r="C108" s="1" t="s">
@@ -1780,7 +1771,7 @@
       <c r="A109" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B109" s="2">
         <v>2</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -1791,7 +1782,7 @@
       <c r="A110" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B110" s="3">
+      <c r="B110" s="2">
         <v>2</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -1802,7 +1793,7 @@
       <c r="A111" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B111" s="3">
+      <c r="B111" s="2">
         <v>2</v>
       </c>
       <c r="C111" s="1" t="s">
@@ -1813,7 +1804,7 @@
       <c r="A112" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B112" s="3">
+      <c r="B112" s="2">
         <v>2</v>
       </c>
       <c r="C112" s="1" t="s">
@@ -1824,18 +1815,18 @@
       <c r="A113" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B113" s="3">
+      <c r="B113" s="2">
         <v>2</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75" hidden="1">
       <c r="A114" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B114" s="2">
         <v>3</v>
       </c>
       <c r="C114" s="1" t="s">
@@ -1846,7 +1837,7 @@
       <c r="A115" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B115" s="2">
         <v>3</v>
       </c>
       <c r="C115" s="1" t="s">
@@ -1857,7 +1848,7 @@
       <c r="A116" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B116" s="3">
+      <c r="B116" s="2">
         <v>3</v>
       </c>
       <c r="C116" s="1" t="s">
@@ -1868,7 +1859,7 @@
       <c r="A117" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B117" s="3">
+      <c r="B117" s="2">
         <v>3</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -1879,7 +1870,7 @@
       <c r="A118" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B118" s="3">
+      <c r="B118" s="2">
         <v>3</v>
       </c>
       <c r="C118" s="1" t="s">
@@ -1890,7 +1881,7 @@
       <c r="A119" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B119" s="3">
+      <c r="B119" s="2">
         <v>3</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -1901,7 +1892,7 @@
       <c r="A120" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B120" s="3">
+      <c r="B120" s="2">
         <v>3</v>
       </c>
       <c r="C120" s="1" t="s">
@@ -1912,7 +1903,7 @@
       <c r="A121" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B121" s="3">
+      <c r="B121" s="2">
         <v>3</v>
       </c>
       <c r="C121" s="1" t="s">
@@ -1923,7 +1914,7 @@
       <c r="A122" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B122" s="3">
+      <c r="B122" s="2">
         <v>3</v>
       </c>
       <c r="C122" s="1" t="s">
@@ -1934,7 +1925,7 @@
       <c r="A123" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B123" s="3">
+      <c r="B123" s="2">
         <v>3</v>
       </c>
       <c r="C123" s="1" t="s">
@@ -1945,7 +1936,7 @@
       <c r="A124" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B124" s="3">
+      <c r="B124" s="2">
         <v>3</v>
       </c>
       <c r="C124" s="1" t="s">
@@ -1956,7 +1947,7 @@
       <c r="A125" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B125" s="3">
+      <c r="B125" s="2">
         <v>3</v>
       </c>
       <c r="C125" s="1" t="s">
@@ -1967,7 +1958,7 @@
       <c r="A126" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B126" s="3">
+      <c r="B126" s="2">
         <v>3</v>
       </c>
       <c r="C126" s="1" t="s">
@@ -1978,7 +1969,7 @@
       <c r="A127" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B127" s="3">
+      <c r="B127" s="2">
         <v>3</v>
       </c>
       <c r="C127" s="1" t="s">
@@ -1989,7 +1980,7 @@
       <c r="A128" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B128" s="3">
+      <c r="B128" s="2">
         <v>3</v>
       </c>
       <c r="C128" s="1" t="s">
@@ -2000,7 +1991,7 @@
       <c r="A129" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B129" s="3">
+      <c r="B129" s="2">
         <v>3</v>
       </c>
       <c r="C129" s="1" t="s">
@@ -2011,7 +2002,7 @@
       <c r="A130" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B130" s="3">
+      <c r="B130" s="2">
         <v>3</v>
       </c>
       <c r="C130" s="1" t="s">
@@ -2022,7 +2013,7 @@
       <c r="A131" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B131" s="3">
+      <c r="B131" s="2">
         <v>3</v>
       </c>
       <c r="C131" s="1" t="s">
@@ -2033,7 +2024,7 @@
       <c r="A132" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B132" s="3">
+      <c r="B132" s="2">
         <v>3</v>
       </c>
       <c r="C132" s="1" t="s">
@@ -2044,7 +2035,7 @@
       <c r="A133" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B133" s="3">
+      <c r="B133" s="2">
         <v>3</v>
       </c>
       <c r="C133" s="1" t="s">
@@ -2055,40 +2046,40 @@
       <c r="A134" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B134" s="3">
+      <c r="B134" s="2">
         <v>3</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75" hidden="1">
       <c r="A135" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B135" s="3">
+      <c r="B135" s="2">
         <v>3</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75" hidden="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B136" s="3">
+      <c r="B136" s="2">
         <v>3</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B137" s="3">
+      <c r="B137" s="2">
         <v>3</v>
       </c>
       <c r="C137" s="1" t="s">
@@ -2099,7 +2090,7 @@
       <c r="A138" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B138" s="3">
+      <c r="B138" s="2">
         <v>3</v>
       </c>
       <c r="C138" s="1" t="s">
@@ -2110,7 +2101,7 @@
       <c r="A139" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B139" s="3">
+      <c r="B139" s="2">
         <v>3</v>
       </c>
       <c r="C139" s="1" t="s">
@@ -2121,7 +2112,7 @@
       <c r="A140" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B140" s="3">
+      <c r="B140" s="2">
         <v>3</v>
       </c>
       <c r="C140" s="1" t="s">
@@ -2132,7 +2123,7 @@
       <c r="A141" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B141" s="3">
+      <c r="B141" s="2">
         <v>3</v>
       </c>
       <c r="C141" s="1" t="s">
@@ -2143,7 +2134,7 @@
       <c r="A142" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B142" s="3">
+      <c r="B142" s="2">
         <v>3</v>
       </c>
       <c r="C142" s="1" t="s">
@@ -2154,7 +2145,7 @@
       <c r="A143" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B143" s="3">
+      <c r="B143" s="2">
         <v>3</v>
       </c>
       <c r="C143" s="1" t="s">
@@ -2165,7 +2156,7 @@
       <c r="A144" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B144" s="3">
+      <c r="B144" s="2">
         <v>3</v>
       </c>
       <c r="C144" s="1" t="s">
@@ -2176,7 +2167,7 @@
       <c r="A145" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B145" s="3">
+      <c r="B145" s="2">
         <v>3</v>
       </c>
       <c r="C145" s="1" t="s">
@@ -2187,7 +2178,7 @@
       <c r="A146" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B146" s="3">
+      <c r="B146" s="2">
         <v>3</v>
       </c>
       <c r="C146" s="1" t="s">
@@ -2198,7 +2189,7 @@
       <c r="A147" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B147" s="3">
+      <c r="B147" s="2">
         <v>3</v>
       </c>
       <c r="C147" s="1" t="s">
@@ -2209,7 +2200,7 @@
       <c r="A148" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B148" s="3">
+      <c r="B148" s="2">
         <v>3</v>
       </c>
       <c r="C148" s="1" t="s">
@@ -2220,7 +2211,7 @@
       <c r="A149" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B149" s="3">
+      <c r="B149" s="2">
         <v>3</v>
       </c>
       <c r="C149" s="1" t="s">
@@ -2231,29 +2222,29 @@
       <c r="A150" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B150" s="3">
+      <c r="B150" s="2">
         <v>3</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75" hidden="1">
       <c r="A151" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B151" s="3">
+      <c r="B151" s="2">
         <v>3</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75" hidden="1">
       <c r="A152" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B152" s="3">
+      <c r="B152" s="2">
         <v>3</v>
       </c>
       <c r="C152" s="1" t="s">
@@ -2264,7 +2255,7 @@
       <c r="A153" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B153" s="3">
+      <c r="B153" s="2">
         <v>3</v>
       </c>
       <c r="C153" s="1" t="s">
@@ -2275,7 +2266,7 @@
       <c r="A154" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B154" s="3">
+      <c r="B154" s="2">
         <v>3</v>
       </c>
       <c r="C154" s="1" t="s">
@@ -2286,7 +2277,7 @@
       <c r="A155" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B155" s="3">
+      <c r="B155" s="2">
         <v>3</v>
       </c>
       <c r="C155" s="1" t="s">
@@ -2297,7 +2288,7 @@
       <c r="A156" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B156" s="3">
+      <c r="B156" s="2">
         <v>3</v>
       </c>
       <c r="C156" s="1" t="s">
@@ -2308,7 +2299,7 @@
       <c r="A157" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B157" s="3">
+      <c r="B157" s="2">
         <v>3</v>
       </c>
       <c r="C157" s="1" t="s">
@@ -2319,7 +2310,7 @@
       <c r="A158" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B158" s="3">
+      <c r="B158" s="2">
         <v>3</v>
       </c>
       <c r="C158" s="1" t="s">
@@ -2330,7 +2321,7 @@
       <c r="A159" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B159" s="3">
+      <c r="B159" s="2">
         <v>3</v>
       </c>
       <c r="C159" s="1" t="s">
@@ -2341,7 +2332,7 @@
       <c r="A160" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B160" s="3">
+      <c r="B160" s="2">
         <v>3</v>
       </c>
       <c r="C160" s="1" t="s">
@@ -2352,7 +2343,7 @@
       <c r="A161" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B161" s="3">
+      <c r="B161" s="2">
         <v>3</v>
       </c>
       <c r="C161" s="1" t="s">
@@ -2363,7 +2354,7 @@
       <c r="A162" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B162" s="3">
+      <c r="B162" s="2">
         <v>3</v>
       </c>
       <c r="C162" s="1" t="s">
@@ -2374,7 +2365,7 @@
       <c r="A163" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B163" s="3">
+      <c r="B163" s="2">
         <v>3</v>
       </c>
       <c r="C163" s="1" t="s">
@@ -2385,7 +2376,7 @@
       <c r="A164" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B164" s="3">
+      <c r="B164" s="2">
         <v>3</v>
       </c>
       <c r="C164" s="1" t="s">
@@ -2396,7 +2387,7 @@
       <c r="A165" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B165" s="3">
+      <c r="B165" s="2">
         <v>3</v>
       </c>
       <c r="C165" s="1" t="s">
@@ -2407,7 +2398,7 @@
       <c r="A166" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B166" s="3">
+      <c r="B166" s="2">
         <v>3</v>
       </c>
       <c r="C166" s="1" t="s">
@@ -2418,7 +2409,7 @@
       <c r="A167" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B167" s="3">
+      <c r="B167" s="2">
         <v>3</v>
       </c>
       <c r="C167" s="1" t="s">
@@ -2429,7 +2420,7 @@
       <c r="A168" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B168" s="3">
+      <c r="B168" s="2">
         <v>3</v>
       </c>
       <c r="C168" s="1" t="s">
@@ -2440,18 +2431,18 @@
       <c r="A169" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B169" s="3">
+      <c r="B169" s="2">
         <v>3</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75" hidden="1">
       <c r="A170" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B170" s="3">
+      <c r="B170" s="2">
         <v>4</v>
       </c>
       <c r="C170" s="1" t="s">
@@ -2462,7 +2453,7 @@
       <c r="A171" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B171" s="3">
+      <c r="B171" s="2">
         <v>4</v>
       </c>
       <c r="C171" s="1" t="s">
@@ -2473,7 +2464,7 @@
       <c r="A172" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B172" s="3">
+      <c r="B172" s="2">
         <v>4</v>
       </c>
       <c r="C172" s="1" t="s">
@@ -2484,7 +2475,7 @@
       <c r="A173" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B173" s="3">
+      <c r="B173" s="2">
         <v>4</v>
       </c>
       <c r="C173" s="1" t="s">
@@ -2495,7 +2486,7 @@
       <c r="A174" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B174" s="3">
+      <c r="B174" s="2">
         <v>4</v>
       </c>
       <c r="C174" s="1" t="s">
@@ -2506,7 +2497,7 @@
       <c r="A175" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B175" s="3">
+      <c r="B175" s="2">
         <v>4</v>
       </c>
       <c r="C175" s="1" t="s">
@@ -2517,7 +2508,7 @@
       <c r="A176" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B176" s="3">
+      <c r="B176" s="2">
         <v>4</v>
       </c>
       <c r="C176" s="1" t="s">
@@ -2528,7 +2519,7 @@
       <c r="A177" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B177" s="3">
+      <c r="B177" s="2">
         <v>4</v>
       </c>
       <c r="C177" s="1" t="s">
@@ -2539,7 +2530,7 @@
       <c r="A178" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B178" s="3">
+      <c r="B178" s="2">
         <v>4</v>
       </c>
       <c r="C178" s="1" t="s">
@@ -2550,7 +2541,7 @@
       <c r="A179" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B179" s="3">
+      <c r="B179" s="2">
         <v>4</v>
       </c>
       <c r="C179" s="1" t="s">
@@ -2561,7 +2552,7 @@
       <c r="A180" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B180" s="3">
+      <c r="B180" s="2">
         <v>4</v>
       </c>
       <c r="C180" s="1" t="s">
@@ -2572,7 +2563,7 @@
       <c r="A181" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B181" s="3">
+      <c r="B181" s="2">
         <v>4</v>
       </c>
       <c r="C181" s="1" t="s">
@@ -2583,7 +2574,7 @@
       <c r="A182" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B182" s="3">
+      <c r="B182" s="2">
         <v>4</v>
       </c>
       <c r="C182" s="1" t="s">
@@ -2594,7 +2585,7 @@
       <c r="A183" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B183" s="3">
+      <c r="B183" s="2">
         <v>4</v>
       </c>
       <c r="C183" s="1" t="s">
@@ -2605,7 +2596,7 @@
       <c r="A184" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B184" s="3">
+      <c r="B184" s="2">
         <v>4</v>
       </c>
       <c r="C184" s="1" t="s">
@@ -2616,7 +2607,7 @@
       <c r="A185" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B185" s="3">
+      <c r="B185" s="2">
         <v>4</v>
       </c>
       <c r="C185" s="1" t="s">
@@ -2627,7 +2618,7 @@
       <c r="A186" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B186" s="3">
+      <c r="B186" s="2">
         <v>4</v>
       </c>
       <c r="C186" s="1" t="s">
@@ -2638,7 +2629,7 @@
       <c r="A187" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B187" s="3">
+      <c r="B187" s="2">
         <v>4</v>
       </c>
       <c r="C187" s="1" t="s">
@@ -2649,7 +2640,7 @@
       <c r="A188" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B188" s="3">
+      <c r="B188" s="2">
         <v>4</v>
       </c>
       <c r="C188" s="1" t="s">
@@ -2660,7 +2651,7 @@
       <c r="A189" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B189" s="3">
+      <c r="B189" s="2">
         <v>4</v>
       </c>
       <c r="C189" s="1" t="s">
@@ -2671,40 +2662,40 @@
       <c r="A190" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B190" s="3">
+      <c r="B190" s="2">
         <v>4</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75" hidden="1">
       <c r="A191" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B191" s="3">
+      <c r="B191" s="2">
         <v>4</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75" hidden="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
       <c r="A192" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B192" s="3">
+      <c r="B192" s="2">
         <v>4</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
       <c r="A193" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B193" s="3">
+      <c r="B193" s="2">
         <v>4</v>
       </c>
       <c r="C193" s="1" t="s">
@@ -2715,7 +2706,7 @@
       <c r="A194" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B194" s="3">
+      <c r="B194" s="2">
         <v>4</v>
       </c>
       <c r="C194" s="1" t="s">
@@ -2726,7 +2717,7 @@
       <c r="A195" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B195" s="3">
+      <c r="B195" s="2">
         <v>4</v>
       </c>
       <c r="C195" s="1" t="s">
@@ -2737,7 +2728,7 @@
       <c r="A196" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B196" s="3">
+      <c r="B196" s="2">
         <v>4</v>
       </c>
       <c r="C196" s="1" t="s">
@@ -2748,7 +2739,7 @@
       <c r="A197" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B197" s="3">
+      <c r="B197" s="2">
         <v>4</v>
       </c>
       <c r="C197" s="1" t="s">
@@ -2759,7 +2750,7 @@
       <c r="A198" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B198" s="3">
+      <c r="B198" s="2">
         <v>4</v>
       </c>
       <c r="C198" s="1" t="s">
@@ -2770,7 +2761,7 @@
       <c r="A199" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B199" s="3">
+      <c r="B199" s="2">
         <v>4</v>
       </c>
       <c r="C199" s="1" t="s">
@@ -2781,7 +2772,7 @@
       <c r="A200" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B200" s="3">
+      <c r="B200" s="2">
         <v>4</v>
       </c>
       <c r="C200" s="1" t="s">
@@ -2792,7 +2783,7 @@
       <c r="A201" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B201" s="3">
+      <c r="B201" s="2">
         <v>4</v>
       </c>
       <c r="C201" s="1" t="s">
@@ -2803,7 +2794,7 @@
       <c r="A202" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B202" s="3">
+      <c r="B202" s="2">
         <v>4</v>
       </c>
       <c r="C202" s="1" t="s">
@@ -2814,7 +2805,7 @@
       <c r="A203" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B203" s="3">
+      <c r="B203" s="2">
         <v>4</v>
       </c>
       <c r="C203" s="1" t="s">
@@ -2825,7 +2816,7 @@
       <c r="A204" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B204" s="3">
+      <c r="B204" s="2">
         <v>4</v>
       </c>
       <c r="C204" s="1" t="s">
@@ -2836,7 +2827,7 @@
       <c r="A205" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B205" s="3">
+      <c r="B205" s="2">
         <v>4</v>
       </c>
       <c r="C205" s="1" t="s">
@@ -2847,29 +2838,29 @@
       <c r="A206" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B206" s="3">
+      <c r="B206" s="2">
         <v>4</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="18.75" hidden="1">
       <c r="A207" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B207" s="3">
+      <c r="B207" s="2">
         <v>4</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="18.75" hidden="1">
       <c r="A208" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B208" s="3">
+      <c r="B208" s="2">
         <v>4</v>
       </c>
       <c r="C208" s="1" t="s">
@@ -2880,7 +2871,7 @@
       <c r="A209" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B209" s="3">
+      <c r="B209" s="2">
         <v>4</v>
       </c>
       <c r="C209" s="1" t="s">
@@ -2891,7 +2882,7 @@
       <c r="A210" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B210" s="3">
+      <c r="B210" s="2">
         <v>4</v>
       </c>
       <c r="C210" s="1" t="s">
@@ -2902,7 +2893,7 @@
       <c r="A211" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B211" s="3">
+      <c r="B211" s="2">
         <v>4</v>
       </c>
       <c r="C211" s="1" t="s">
@@ -2913,7 +2904,7 @@
       <c r="A212" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B212" s="3">
+      <c r="B212" s="2">
         <v>4</v>
       </c>
       <c r="C212" s="1" t="s">
@@ -2924,7 +2915,7 @@
       <c r="A213" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B213" s="3">
+      <c r="B213" s="2">
         <v>4</v>
       </c>
       <c r="C213" s="1" t="s">
@@ -2935,7 +2926,7 @@
       <c r="A214" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B214" s="3">
+      <c r="B214" s="2">
         <v>4</v>
       </c>
       <c r="C214" s="1" t="s">
@@ -2946,7 +2937,7 @@
       <c r="A215" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B215" s="3">
+      <c r="B215" s="2">
         <v>4</v>
       </c>
       <c r="C215" s="1" t="s">
@@ -2957,7 +2948,7 @@
       <c r="A216" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B216" s="3">
+      <c r="B216" s="2">
         <v>4</v>
       </c>
       <c r="C216" s="1" t="s">
@@ -2968,7 +2959,7 @@
       <c r="A217" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B217" s="3">
+      <c r="B217" s="2">
         <v>4</v>
       </c>
       <c r="C217" s="1" t="s">
@@ -2979,7 +2970,7 @@
       <c r="A218" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B218" s="3">
+      <c r="B218" s="2">
         <v>4</v>
       </c>
       <c r="C218" s="1" t="s">
@@ -2990,7 +2981,7 @@
       <c r="A219" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B219" s="3">
+      <c r="B219" s="2">
         <v>4</v>
       </c>
       <c r="C219" s="1" t="s">
@@ -3001,7 +2992,7 @@
       <c r="A220" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B220" s="3">
+      <c r="B220" s="2">
         <v>4</v>
       </c>
       <c r="C220" s="1" t="s">
@@ -3012,7 +3003,7 @@
       <c r="A221" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B221" s="3">
+      <c r="B221" s="2">
         <v>4</v>
       </c>
       <c r="C221" s="1" t="s">
@@ -3023,7 +3014,7 @@
       <c r="A222" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B222" s="3">
+      <c r="B222" s="2">
         <v>4</v>
       </c>
       <c r="C222" s="1" t="s">
@@ -3034,7 +3025,7 @@
       <c r="A223" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B223" s="3">
+      <c r="B223" s="2">
         <v>4</v>
       </c>
       <c r="C223" s="1" t="s">
@@ -3045,7 +3036,7 @@
       <c r="A224" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B224" s="3">
+      <c r="B224" s="2">
         <v>4</v>
       </c>
       <c r="C224" s="1" t="s">
@@ -3056,18 +3047,18 @@
       <c r="A225" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B225" s="3">
+      <c r="B225" s="2">
         <v>4</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="18.75" hidden="1">
       <c r="A226" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B226" s="3">
+      <c r="B226" s="2">
         <v>5</v>
       </c>
       <c r="C226" s="1" t="s">
@@ -3078,7 +3069,7 @@
       <c r="A227" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B227" s="3">
+      <c r="B227" s="2">
         <v>5</v>
       </c>
       <c r="C227" s="1" t="s">
@@ -3089,7 +3080,7 @@
       <c r="A228" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B228" s="3">
+      <c r="B228" s="2">
         <v>5</v>
       </c>
       <c r="C228" s="1" t="s">
@@ -3100,7 +3091,7 @@
       <c r="A229" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B229" s="3">
+      <c r="B229" s="2">
         <v>5</v>
       </c>
       <c r="C229" s="1" t="s">
@@ -3111,7 +3102,7 @@
       <c r="A230" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B230" s="3">
+      <c r="B230" s="2">
         <v>5</v>
       </c>
       <c r="C230" s="1" t="s">
@@ -3122,7 +3113,7 @@
       <c r="A231" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B231" s="3">
+      <c r="B231" s="2">
         <v>5</v>
       </c>
       <c r="C231" s="1" t="s">
@@ -3133,7 +3124,7 @@
       <c r="A232" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B232" s="3">
+      <c r="B232" s="2">
         <v>5</v>
       </c>
       <c r="C232" s="1" t="s">
@@ -3144,7 +3135,7 @@
       <c r="A233" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B233" s="3">
+      <c r="B233" s="2">
         <v>5</v>
       </c>
       <c r="C233" s="1" t="s">
@@ -3155,7 +3146,7 @@
       <c r="A234" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B234" s="3">
+      <c r="B234" s="2">
         <v>5</v>
       </c>
       <c r="C234" s="1" t="s">
@@ -3166,7 +3157,7 @@
       <c r="A235" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B235" s="3">
+      <c r="B235" s="2">
         <v>5</v>
       </c>
       <c r="C235" s="1" t="s">
@@ -3177,7 +3168,7 @@
       <c r="A236" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B236" s="3">
+      <c r="B236" s="2">
         <v>5</v>
       </c>
       <c r="C236" s="1" t="s">
@@ -3188,7 +3179,7 @@
       <c r="A237" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B237" s="3">
+      <c r="B237" s="2">
         <v>5</v>
       </c>
       <c r="C237" s="1" t="s">
@@ -3199,7 +3190,7 @@
       <c r="A238" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B238" s="3">
+      <c r="B238" s="2">
         <v>5</v>
       </c>
       <c r="C238" s="1" t="s">
@@ -3210,7 +3201,7 @@
       <c r="A239" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B239" s="3">
+      <c r="B239" s="2">
         <v>5</v>
       </c>
       <c r="C239" s="1" t="s">
@@ -3221,7 +3212,7 @@
       <c r="A240" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B240" s="3">
+      <c r="B240" s="2">
         <v>5</v>
       </c>
       <c r="C240" s="1" t="s">
@@ -3232,7 +3223,7 @@
       <c r="A241" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B241" s="3">
+      <c r="B241" s="2">
         <v>5</v>
       </c>
       <c r="C241" s="1" t="s">
@@ -3243,7 +3234,7 @@
       <c r="A242" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B242" s="3">
+      <c r="B242" s="2">
         <v>5</v>
       </c>
       <c r="C242" s="1" t="s">
@@ -3254,7 +3245,7 @@
       <c r="A243" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B243" s="3">
+      <c r="B243" s="2">
         <v>5</v>
       </c>
       <c r="C243" s="1" t="s">
@@ -3265,7 +3256,7 @@
       <c r="A244" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B244" s="3">
+      <c r="B244" s="2">
         <v>5</v>
       </c>
       <c r="C244" s="1" t="s">
@@ -3276,7 +3267,7 @@
       <c r="A245" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B245" s="3">
+      <c r="B245" s="2">
         <v>5</v>
       </c>
       <c r="C245" s="1" t="s">
@@ -3287,40 +3278,40 @@
       <c r="A246" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B246" s="3">
+      <c r="B246" s="2">
         <v>5</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="18.75" hidden="1">
       <c r="A247" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B247" s="3">
+      <c r="B247" s="2">
         <v>5</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="18.75" hidden="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="18.75">
       <c r="A248" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B248" s="3">
+      <c r="B248" s="2">
         <v>5</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="18.75">
       <c r="A249" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B249" s="3">
+      <c r="B249" s="2">
         <v>5</v>
       </c>
       <c r="C249" s="1" t="s">
@@ -3331,7 +3322,7 @@
       <c r="A250" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B250" s="3">
+      <c r="B250" s="2">
         <v>5</v>
       </c>
       <c r="C250" s="1" t="s">
@@ -3342,7 +3333,7 @@
       <c r="A251" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B251" s="3">
+      <c r="B251" s="2">
         <v>5</v>
       </c>
       <c r="C251" s="1" t="s">
@@ -3353,7 +3344,7 @@
       <c r="A252" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B252" s="3">
+      <c r="B252" s="2">
         <v>5</v>
       </c>
       <c r="C252" s="1" t="s">
@@ -3364,7 +3355,7 @@
       <c r="A253" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B253" s="3">
+      <c r="B253" s="2">
         <v>5</v>
       </c>
       <c r="C253" s="1" t="s">
@@ -3375,7 +3366,7 @@
       <c r="A254" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B254" s="3">
+      <c r="B254" s="2">
         <v>5</v>
       </c>
       <c r="C254" s="1" t="s">
@@ -3386,7 +3377,7 @@
       <c r="A255" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B255" s="3">
+      <c r="B255" s="2">
         <v>5</v>
       </c>
       <c r="C255" s="1" t="s">
@@ -3397,7 +3388,7 @@
       <c r="A256" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B256" s="3">
+      <c r="B256" s="2">
         <v>5</v>
       </c>
       <c r="C256" s="1" t="s">
@@ -3408,7 +3399,7 @@
       <c r="A257" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B257" s="3">
+      <c r="B257" s="2">
         <v>5</v>
       </c>
       <c r="C257" s="1" t="s">
@@ -3419,7 +3410,7 @@
       <c r="A258" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B258" s="3">
+      <c r="B258" s="2">
         <v>5</v>
       </c>
       <c r="C258" s="1" t="s">
@@ -3430,7 +3421,7 @@
       <c r="A259" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B259" s="3">
+      <c r="B259" s="2">
         <v>5</v>
       </c>
       <c r="C259" s="1" t="s">
@@ -3441,7 +3432,7 @@
       <c r="A260" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B260" s="3">
+      <c r="B260" s="2">
         <v>5</v>
       </c>
       <c r="C260" s="1" t="s">
@@ -3452,7 +3443,7 @@
       <c r="A261" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B261" s="3">
+      <c r="B261" s="2">
         <v>5</v>
       </c>
       <c r="C261" s="1" t="s">
@@ -3463,29 +3454,29 @@
       <c r="A262" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B262" s="3">
+      <c r="B262" s="2">
         <v>5</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="263" customHeight="1" ht="18.75" hidden="1">
       <c r="A263" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B263" s="3">
+      <c r="B263" s="2">
         <v>5</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="264" customHeight="1" ht="18.75" hidden="1">
       <c r="A264" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B264" s="3">
+      <c r="B264" s="2">
         <v>5</v>
       </c>
       <c r="C264" s="1" t="s">
@@ -3496,7 +3487,7 @@
       <c r="A265" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B265" s="3">
+      <c r="B265" s="2">
         <v>5</v>
       </c>
       <c r="C265" s="1" t="s">
@@ -3507,7 +3498,7 @@
       <c r="A266" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B266" s="3">
+      <c r="B266" s="2">
         <v>5</v>
       </c>
       <c r="C266" s="1" t="s">
@@ -3518,7 +3509,7 @@
       <c r="A267" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B267" s="3">
+      <c r="B267" s="2">
         <v>5</v>
       </c>
       <c r="C267" s="1" t="s">
@@ -3529,7 +3520,7 @@
       <c r="A268" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B268" s="3">
+      <c r="B268" s="2">
         <v>5</v>
       </c>
       <c r="C268" s="1" t="s">
@@ -3540,7 +3531,7 @@
       <c r="A269" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B269" s="3">
+      <c r="B269" s="2">
         <v>5</v>
       </c>
       <c r="C269" s="1" t="s">
@@ -3551,7 +3542,7 @@
       <c r="A270" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B270" s="3">
+      <c r="B270" s="2">
         <v>5</v>
       </c>
       <c r="C270" s="1" t="s">
@@ -3562,7 +3553,7 @@
       <c r="A271" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B271" s="3">
+      <c r="B271" s="2">
         <v>5</v>
       </c>
       <c r="C271" s="1" t="s">
@@ -3573,7 +3564,7 @@
       <c r="A272" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B272" s="3">
+      <c r="B272" s="2">
         <v>5</v>
       </c>
       <c r="C272" s="1" t="s">
@@ -3584,7 +3575,7 @@
       <c r="A273" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B273" s="3">
+      <c r="B273" s="2">
         <v>5</v>
       </c>
       <c r="C273" s="1" t="s">
@@ -3595,7 +3586,7 @@
       <c r="A274" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B274" s="3">
+      <c r="B274" s="2">
         <v>5</v>
       </c>
       <c r="C274" s="1" t="s">
@@ -3606,7 +3597,7 @@
       <c r="A275" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B275" s="3">
+      <c r="B275" s="2">
         <v>5</v>
       </c>
       <c r="C275" s="1" t="s">
@@ -3617,7 +3608,7 @@
       <c r="A276" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B276" s="3">
+      <c r="B276" s="2">
         <v>5</v>
       </c>
       <c r="C276" s="1" t="s">
@@ -3628,7 +3619,7 @@
       <c r="A277" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B277" s="3">
+      <c r="B277" s="2">
         <v>5</v>
       </c>
       <c r="C277" s="1" t="s">
@@ -3639,7 +3630,7 @@
       <c r="A278" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B278" s="3">
+      <c r="B278" s="2">
         <v>5</v>
       </c>
       <c r="C278" s="1" t="s">
@@ -3650,7 +3641,7 @@
       <c r="A279" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B279" s="3">
+      <c r="B279" s="2">
         <v>5</v>
       </c>
       <c r="C279" s="1" t="s">
@@ -3661,7 +3652,7 @@
       <c r="A280" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B280" s="3">
+      <c r="B280" s="2">
         <v>5</v>
       </c>
       <c r="C280" s="1" t="s">
@@ -3672,7 +3663,7 @@
       <c r="A281" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B281" s="3">
+      <c r="B281" s="2">
         <v>5</v>
       </c>
       <c r="C281" s="1" t="s">

</xml_diff>

<commit_message>
pago hasta el 10 de agosto
</commit_message>
<xml_diff>
--- a/DATA/Pagos.xlsx
+++ b/DATA/Pagos.xlsx
@@ -832,7 +832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" hidden="1">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -843,7 +843,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" hidden="1">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -942,7 +942,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -950,10 +950,10 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" hidden="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -961,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" hidden="1">
@@ -1448,7 +1448,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75" hidden="1">
       <c r="A80" s="1" t="s">
         <v>27</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75" hidden="1">
       <c r="A81" s="1" t="s">
         <v>28</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="1" t="s">
         <v>37</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="1" t="s">
         <v>38</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75" hidden="1">
       <c r="A136" s="1" t="s">
         <v>27</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75" hidden="1">
       <c r="A137" s="1" t="s">
         <v>28</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="1" t="s">
         <v>37</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="1" t="s">
         <v>38</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75" hidden="1">
       <c r="A192" s="1" t="s">
         <v>27</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75" hidden="1">
       <c r="A193" s="1" t="s">
         <v>28</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75">
       <c r="A202" s="1" t="s">
         <v>37</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75">
       <c r="A203" s="1" t="s">
         <v>38</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="18.75" hidden="1">
       <c r="A248" s="1" t="s">
         <v>27</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="18.75" hidden="1">
       <c r="A249" s="1" t="s">
         <v>28</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="18.75">
       <c r="A258" s="1" t="s">
         <v>37</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="18.75">
       <c r="A259" s="1" t="s">
         <v>38</v>
       </c>

</xml_diff>